<commit_message>
pequenas atualizações na documentação e backlog
</commit_message>
<xml_diff>
--- a/Documentos/Backlog.xlsx
+++ b/Documentos/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sptech\Documents\Cars life\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sptech\Documents\CarsLife\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC746E9-6868-4760-80ED-EC7FF80C61D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDE9EE2-8444-442A-909B-DD3944579825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
   <si>
     <t>Status</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t xml:space="preserve">Feitos: </t>
-  </si>
-  <si>
-    <t>Pendente</t>
   </si>
   <si>
     <t xml:space="preserve">Pendentes: </t>
@@ -1051,10 +1048,10 @@
                   <c:v>Pendentes: </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1066,10 +1063,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2145,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CE1519-2D3C-4AEF-AD18-290FC829BB4D}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C2" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2192,16 +2189,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="11">
         <f t="shared" ref="F3:F48" si="0">IF(E3="PP", 3, IF(E3="P", 5, IF(E3="M", 8, IF(E3="G", 13, IF(E3="GG", 21, "")))))</f>
@@ -2216,7 +2213,7 @@
       </c>
       <c r="K3" s="16">
         <f>COUNTIF(Tabela2[[#All],[Status]], "feito")</f>
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2224,16 +2221,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="11">
         <f t="shared" si="0"/>
@@ -2244,11 +2241,11 @@
       </c>
       <c r="I4" s="19"/>
       <c r="J4" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" s="16">
         <f>COUNTIF(Tabela2[[#All],[Status]], "pendente")</f>
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2256,16 +2253,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>36</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="11">
         <f t="shared" si="0"/>
@@ -2279,19 +2276,19 @@
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="11">
         <f t="shared" si="0"/>
@@ -2305,19 +2302,19 @@
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="11">
         <f t="shared" si="0"/>
@@ -2331,19 +2328,19 @@
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="21" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="11">
         <f t="shared" si="0"/>
@@ -2355,19 +2352,19 @@
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>43</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>44</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="11">
         <f t="shared" si="0"/>
@@ -2382,16 +2379,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>48</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="11">
         <f t="shared" si="0"/>
@@ -2403,19 +2400,19 @@
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="21" t="s">
         <v>45</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>46</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="11">
         <f t="shared" si="0"/>
@@ -2427,19 +2424,19 @@
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>50</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>51</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="11">
         <f t="shared" si="0"/>
@@ -2451,19 +2448,19 @@
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>52</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>53</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="11">
         <f t="shared" si="0"/>
@@ -2475,19 +2472,19 @@
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>54</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>55</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="11">
         <f t="shared" si="0"/>
@@ -2499,19 +2496,19 @@
     </row>
     <row r="15" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>56</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="11">
         <f t="shared" si="0"/>
@@ -2523,19 +2520,19 @@
     </row>
     <row r="16" spans="1:11" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>58</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>59</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="11">
         <f t="shared" si="0"/>
@@ -2547,19 +2544,19 @@
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>61</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F17" s="11">
         <f t="shared" si="0"/>
@@ -2571,19 +2568,19 @@
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>63</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>64</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="11">
         <f t="shared" si="0"/>
@@ -2595,19 +2592,19 @@
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="22" t="s">
         <v>65</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>66</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F19" s="23">
         <f t="shared" si="0"/>
@@ -2619,19 +2616,19 @@
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F20" s="32">
         <f t="shared" si="0"/>
@@ -2995,7 +2992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D393639F-A27B-4720-9E3A-80DF01992987}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3006,84 +3003,84 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
       <c r="F1" s="35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>20</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="E4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>73</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3096,6 +3093,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1dc861b8-2196-455d-b291-a999da8cffb6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045B33021656A9E479DF12B9A8EE42828" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="17fbaa8b78f929e9c1b60b452d801ff5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1dc861b8-2196-455d-b291-a999da8cffb6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98d66f644378763448046a9d467192f6" ns3:_="">
     <xsd:import namespace="1dc861b8-2196-455d-b291-a999da8cffb6"/>
@@ -3277,24 +3291,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE64FA08-4910-4958-8231-425E1FEB5D81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1dc861b8-2196-455d-b291-a999da8cffb6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1dc861b8-2196-455d-b291-a999da8cffb6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38453624-7FFF-45CC-98E3-4055FC26EDB0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF0E4B6-F289-4603-9B40-4B4593294006}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3310,28 +3331,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38453624-7FFF-45CC-98E3-4055FC26EDB0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE64FA08-4910-4958-8231-425E1FEB5D81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="1dc861b8-2196-455d-b291-a999da8cffb6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>